<commit_message>
feat: enhance test UI and career analysis documentation
- Simplify OptionButton interaction: replaced double-tap unselect with single-click toggle for better UX.
- Update career_analysis.xlsx: added detailed algorithmic impact for Edustats and Vibematch questions, including new logic for family sentiment (e_08) and Likert scale (1-5).
- (Docs) Updated Matrix with descriptive headers and logic breakdown.
</commit_message>
<xml_diff>
--- a/career_analysis.xlsx
+++ b/career_analysis.xlsx
@@ -3169,7 +3169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3180,7 +3180,8 @@
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="60" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="52" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3201,6 +3202,11 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Algorithmic Impact</t>
         </is>
       </c>
@@ -3223,7 +3229,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Maps to {'R': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Maps to {'R': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3256,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Maps to {'C': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Maps to {'C': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3283,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Maps to {'I': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Maps to {'I': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3310,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Maps to {'S': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Maps to {'S': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3337,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Maps to {'A': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Maps to {'A': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3364,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Maps to {'E': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Maps to {'E': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3391,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Maps to {'C': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Maps to {'C': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3418,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Maps to {'R': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Maps to {'R': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3445,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Maps to {'I': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Maps to {'I': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3472,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Maps to {'A': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Maps to {'A': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3499,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Maps to {'C': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Maps to {'C': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3526,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Maps to {'S': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Maps to {'S': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3553,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Maps to {'E': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Maps to {'E': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3580,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Maps to {'I': 1}. Contributes to 40% RIASEC Score.</t>
+          <t>Strongly Disagree (1), Disagree (2), Neutral (3), Agree (4), Strongly Agree (5)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Maps to {'I': 1}. Score (1-5) weighted by 40% RIASEC component.</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3607,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Maps to {}. Contributes to 40% RIASEC Score.</t>
+          <t>Text Response</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Scoring (Practical): Bonus if text matches career/bucket (Positive Reinforcement).</t>
         </is>
       </c>
     </row>

</xml_diff>